<commit_message>
Ghi ten bai hoc
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A7B7E-01CA-4559-A546-80622A25D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B3918-1F40-4BF5-ABE8-555E6D1C6E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>Thời gian</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Nguyễn Lê Phương Nguyên</t>
   </si>
 </sst>
 </file>
@@ -535,54 +538,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ghi ten bai học ten lop
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B3918-1F40-4BF5-ABE8-555E6D1C6E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416CA79-4E4F-4581-935E-439714306AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>Thời gian</t>
   </si>
@@ -161,7 +161,19 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Nguyễn Lê Phương Nguyên</t>
+    <t>1/7</t>
+  </si>
+  <si>
+    <t>1/8</t>
+  </si>
+  <si>
+    <t>1/9</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>phuong nguyen</t>
   </si>
 </sst>
 </file>
@@ -197,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -538,22 +551,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
them ten lop va bai dung vi tri
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416CA79-4E4F-4581-935E-439714306AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D285EE-E689-4988-B01F-D1041430AF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
   <si>
     <t>Thời gian</t>
   </si>
@@ -161,19 +161,10 @@
     <t>abc</t>
   </si>
   <si>
-    <t>1/7</t>
-  </si>
-  <si>
-    <t>1/8</t>
-  </si>
-  <si>
-    <t>1/9</t>
-  </si>
-  <si>
-    <t>1/2</t>
-  </si>
-  <si>
-    <t>phuong nguyen</t>
+    <t>2/1</t>
+  </si>
+  <si>
+    <t>phương nguyên</t>
   </si>
 </sst>
 </file>
@@ -561,48 +552,33 @@
       <c r="A1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update teacher update read_file
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D285EE-E689-4988-B01F-D1041430AF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC0289B-9B27-4375-8E4D-D0DE6B5E116D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>Thời gian</t>
   </si>
@@ -161,10 +161,13 @@
     <t>abc</t>
   </si>
   <si>
-    <t>2/1</t>
-  </si>
-  <si>
-    <t>phương nguyên</t>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>test teacher</t>
+  </si>
+  <si>
+    <t>Cô Nguyên</t>
   </si>
 </sst>
 </file>
@@ -542,43 +545,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sheet rename sheet
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,20 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F11092D-0F4A-4516-A8C5-EF062691FA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B11E2B-E2B9-421C-A7AC-7B36A56073DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="7.9.2022" sheetId="3" r:id="rId1"/>
-    <sheet name="Trang_tính1" sheetId="2" r:id="rId2"/>
+    <sheet name="Tuan 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Tuần 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Trang_tính1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="52">
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>3/4</t>
+  </si>
+  <si>
+    <t>dfd</t>
+  </si>
+  <si>
+    <t>Thầy kiệt</t>
+  </si>
+  <si>
+    <t>2/1</t>
+  </si>
+  <si>
+    <t>cong hoa</t>
+  </si>
+  <si>
+    <t>Cô Nguyên</t>
+  </si>
   <si>
     <t>Thời gian</t>
   </si>
@@ -77,9 +99,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>3/4</t>
-  </si>
-  <si>
     <t>Thứ 3.2</t>
   </si>
   <si>
@@ -158,16 +177,7 @@
     <t>CN</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>3/9</t>
-  </si>
-  <si>
-    <t>sdfdfdfd</t>
-  </si>
-  <si>
-    <t>Cô Nguyên</t>
+    <t>con</t>
   </si>
 </sst>
 </file>
@@ -544,39 +554,446 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75E0ACD-B550-4ECF-A505-7E850879C6CA}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C694C321-98A1-47A6-8345-0974EAEFBFB0}">
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
+      <c r="E45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -585,8 +1002,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:D2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,139 +1069,121 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,228 +1191,321 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
       <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
         <v>30</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>43</v>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
         <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G40" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G55" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
them dung vi tri cua cac truong
</commit_message>
<xml_diff>
--- a/theodoipm_v3/theodoiphongmay.xlsx
+++ b/theodoipm_v3/theodoiphongmay.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\theodoipm_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A96E9C-9AE7-4238-820F-605A04B71CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3306A959-6B8F-4858-ACE5-22F3A3DB9C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tuần 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Tuần 3" sheetId="2" r:id="rId1"/>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="50">
   <si>
     <t>Thời gian</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Tiết</t>
   </si>
   <si>
-    <t>Thứ 2.3</t>
+    <t>Thứ 2</t>
   </si>
   <si>
     <t>1</t>
@@ -80,7 +80,7 @@
     <t>3/4</t>
   </si>
   <si>
-    <t>Thứ 3.2</t>
+    <t>Thứ 3</t>
   </si>
   <si>
     <t>3/5</t>
@@ -156,6 +156,21 @@
   </si>
   <si>
     <t>CN</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>test vi tri v3</t>
+  </si>
+  <si>
+    <t>Cô Nguyên</t>
   </si>
 </sst>
 </file>
@@ -191,8 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -531,14 +547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA31D248-F6FB-4DB2-8A68-E63E568CAE4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC994205-F1BE-44AF-A5CD-395E4DCE6776}">
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -566,7 +582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -574,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -585,7 +601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -596,7 +612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -607,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -618,32 +634,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -657,7 +673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -668,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -679,7 +695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -690,22 +706,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>13</v>
       </c>
@@ -716,17 +732,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -740,7 +756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -751,7 +767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -762,7 +778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -773,27 +789,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -804,26 +820,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C33" t="s">
-        <v>33</v>
+      <c r="C33" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -834,18 +853,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>13</v>
       </c>
-      <c r="C35" t="s">
-        <v>36</v>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>15</v>
       </c>
@@ -856,22 +878,40 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>13</v>
       </c>
@@ -882,17 +922,26 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -906,7 +955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -917,7 +966,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>13</v>
       </c>
@@ -928,47 +977,47 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -984,9 +1033,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1022,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -1055,7 +1104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1066,32 +1115,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -1127,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1138,22 +1187,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>13</v>
       </c>
@@ -1164,17 +1213,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1188,7 +1237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -1210,7 +1259,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -1221,27 +1270,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -1252,12 +1301,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1271,7 +1320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1331,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>13</v>
       </c>
@@ -1293,7 +1342,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>15</v>
       </c>
@@ -1304,22 +1353,22 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>13</v>
       </c>
@@ -1330,17 +1379,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1354,7 +1403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -1365,7 +1414,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>13</v>
       </c>
@@ -1376,47 +1425,47 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>

</xml_diff>